<commit_message>
Add SQL analysis queries for sales performance insights
</commit_message>
<xml_diff>
--- a/excel/sales_report.xlsx
+++ b/excel/sales_report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7270" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales by Product Category" sheetId="2" r:id="rId1"/>
@@ -23272,7 +23272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -23332,7 +23332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -23600,7 +23600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A984" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E993" sqref="E993"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enhance README with professional project documentation
</commit_message>
<xml_diff>
--- a/excel/sales_report.xlsx
+++ b/excel/sales_report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7270" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7270" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sales by Product Category" sheetId="2" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Sales by Age Group" sheetId="5" r:id="rId4"/>
     <sheet name="cleaned_sales" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -3742,7 +3742,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3996,7 +3995,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4158,6 +4156,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4320,7 +4321,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -22692,7 +22692,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -22760,7 +22760,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -22868,7 +22868,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -22932,7 +22932,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -23332,7 +23332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -23600,7 +23600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E993" sqref="E993"/>
     </sheetView>
   </sheetViews>

</xml_diff>